<commit_message>
wip: adding view for skills/items, added core and main fields with modulation
</commit_message>
<xml_diff>
--- a/assets/translation/text.xlsx
+++ b/assets/translation/text.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanMovchanets\Documents\tower-dungeon\assets\translation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\assets\translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF244BB-C96B-4DDD-A9E9-ACEA412A0F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A890A4E5-A06D-45AD-8DD6-787F87FA3833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="3804" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="text" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
   <si>
     <t>key</t>
   </si>
@@ -52,7 +52,301 @@
     <t>Привіт</t>
   </si>
   <si>
-    <t>Laabas</t>
+    <t>Labas</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Назва</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Опис</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Значення</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Швидкість</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Відстань</t>
+  </si>
+  <si>
+    <t>energy_cost</t>
+  </si>
+  <si>
+    <t>Energy Cost</t>
+  </si>
+  <si>
+    <t>Вартість енергії</t>
+  </si>
+  <si>
+    <t>cast_time</t>
+  </si>
+  <si>
+    <t>Cast Time</t>
+  </si>
+  <si>
+    <t>Час виклику</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Тривалість</t>
+  </si>
+  <si>
+    <t>cooldown</t>
+  </si>
+  <si>
+    <t>Cooldown</t>
+  </si>
+  <si>
+    <t>Час до готовності</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Ціна</t>
+  </si>
+  <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Навичка</t>
+  </si>
+  <si>
+    <t>base_value</t>
+  </si>
+  <si>
+    <t>Base Value</t>
+  </si>
+  <si>
+    <t>Базове Значення</t>
+  </si>
+  <si>
+    <t>base_speed</t>
+  </si>
+  <si>
+    <t>Base Speed</t>
+  </si>
+  <si>
+    <t>Базова швидкість</t>
+  </si>
+  <si>
+    <t>base_distance</t>
+  </si>
+  <si>
+    <t>Base Distance</t>
+  </si>
+  <si>
+    <t>Базова відстань</t>
+  </si>
+  <si>
+    <t>base_energy_cost</t>
+  </si>
+  <si>
+    <t>Base Energy Cost</t>
+  </si>
+  <si>
+    <t>Базові вартість енергії</t>
+  </si>
+  <si>
+    <t>base_cast_time</t>
+  </si>
+  <si>
+    <t>Base Cast Time</t>
+  </si>
+  <si>
+    <t>Базовий час виклику</t>
+  </si>
+  <si>
+    <t>base_duration</t>
+  </si>
+  <si>
+    <t>Base Duration</t>
+  </si>
+  <si>
+    <t>Базова тривалість</t>
+  </si>
+  <si>
+    <t>base_cooldown</t>
+  </si>
+  <si>
+    <t>Base Cooldown</t>
+  </si>
+  <si>
+    <t>Базовий час до готовності</t>
+  </si>
+  <si>
+    <t>skill_price</t>
+  </si>
+  <si>
+    <t>Skill Price</t>
+  </si>
+  <si>
+    <t>Базова ціна</t>
+  </si>
+  <si>
+    <t>skill_upgrade</t>
+  </si>
+  <si>
+    <t>Skill Upgrade</t>
+  </si>
+  <si>
+    <t>Покращення навички</t>
+  </si>
+  <si>
+    <t>parameter_name</t>
+  </si>
+  <si>
+    <t>Parameter Name</t>
+  </si>
+  <si>
+    <t>Назва параметру</t>
+  </si>
+  <si>
+    <t>max_lvl</t>
+  </si>
+  <si>
+    <t>Max level</t>
+  </si>
+  <si>
+    <t>Максимальний рівень</t>
+  </si>
+  <si>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>Іскра</t>
+  </si>
+  <si>
+    <t>Kibirkštis</t>
+  </si>
+  <si>
+    <t>spark_skill_description</t>
+  </si>
+  <si>
+    <t>Spark is esential skill of every wizard. Be like Zeus throw yout sparks on your enemies!</t>
+  </si>
+  <si>
+    <t>Іскра - базован навичка гожного мага. Будь як Зевс, закидай ворогів іскрами!</t>
+  </si>
+  <si>
+    <t>Kibirkštis yra pagrindinis kiekvieno mago įgūdis. Būkite kaip Zeusas, meskite kibirkštis į savo priešus!</t>
+  </si>
+  <si>
+    <t>aim_skill_description</t>
+  </si>
+  <si>
+    <t>spark_skill_title</t>
+  </si>
+  <si>
+    <t>aim_skill_title</t>
+  </si>
+  <si>
+    <t>Zoom in</t>
+  </si>
+  <si>
+    <t>Приближення</t>
+  </si>
+  <si>
+    <t>Allows player to zoom in enemies and other objects. Uses stamina as main resourse. Good to see you enemies from big distances.</t>
+  </si>
+  <si>
+    <t>Дозволяє гравцеві збільшувати масштаб ворогів та інших об'єктів. Використовує витривалість як основний ресурс. Приємно бачити ворогів з великої відстані.</t>
+  </si>
+  <si>
+    <t>Leidžia žaidėjui priartinti priešus ir kitus objektus. Naudoja ištvermę kaip pagrindinį resursą. Smagu matyti jus priešus iš didelių atstumų.</t>
+  </si>
+  <si>
+    <t>Priartinti</t>
+  </si>
+  <si>
+    <t>how_to_use_maintainable</t>
+  </si>
+  <si>
+    <t>how_to_use_click_consumable</t>
+  </si>
+  <si>
+    <t>how_to_use_click</t>
+  </si>
+  <si>
+    <t>Click and hold mouse button when item in hands (LMB for left hand / RMB for right hand).</t>
+  </si>
+  <si>
+    <t>Spustelėkite ir laikykite pelės mygtuką, kai daiktas yra rankose (LMB kairiajai rankai / RMB dešinei rankai).</t>
+  </si>
+  <si>
+    <t>Натисніть і утримуйте кнопку миші, коли предмет у руках (ЛКМ для лівої руки / ПКМ для правої руки).</t>
+  </si>
+  <si>
+    <t>Click LMB or RMB to use when item in one of your hands.</t>
+  </si>
+  <si>
+    <t>Клацніть ЛКМ або ПКМ, щоб використати предмет у своїх руках.</t>
+  </si>
+  <si>
+    <t>Spustelėkite LMB arba RMB, kad naudotumėte, kai prekė yra vienoje iš jūsų rankų.</t>
+  </si>
+  <si>
+    <t>Click LMB or RMB to use when item in one of your hands. Item will be consumed after usage!</t>
+  </si>
+  <si>
+    <t>Клацніть ЛКМ або ПКМ, щоб використати предмет у своїх руках. Предмет буде спожито після використання!</t>
+  </si>
+  <si>
+    <t>Spustelėkite LMB arba RMB, kad naudotumėte, kai prekė yra vienoje iš jūsų rankų. Daiktas bus sunaudota po naudojimo!</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Кількість</t>
+  </si>
+  <si>
+    <t>Kiekis</t>
   </si>
 </sst>
 </file>
@@ -536,13 +830,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -919,29 +1210,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -955,7 +1252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -969,7 +1266,362 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>94</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add stone item, skill
</commit_message>
<xml_diff>
--- a/assets/translation/text.xlsx
+++ b/assets/translation/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\assets\translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A890A4E5-A06D-45AD-8DD6-787F87FA3833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E250CA-2E38-445C-B6B1-D226AA644256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="text" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
   <si>
     <t>key</t>
   </si>
@@ -347,6 +347,30 @@
   </si>
   <si>
     <t>Kiekis</t>
+  </si>
+  <si>
+    <t>stone_skill_title</t>
+  </si>
+  <si>
+    <t>stone_skill_description</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Akmenis</t>
+  </si>
+  <si>
+    <t>Камінчик</t>
+  </si>
+  <si>
+    <t>Stones are usefull for building or throwing it. Please try not to throw all of them they are more usefull for small buildings.</t>
+  </si>
+  <si>
+    <t>Камінці корисні для будівництва або кидання. Будь ласка, намагайтеся не викидати їх усі, вони більш корисні для невеликих будівель.</t>
+  </si>
+  <si>
+    <t>Akmenys naudingi statant ar mėtant. Stenkitės neišmesti jų visų, jie yra naudingesni mažiems pastatams.</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,71 +1576,99 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add crystal item, skill, controller - looks good
</commit_message>
<xml_diff>
--- a/assets/translation/text.xlsx
+++ b/assets/translation/text.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\assets\translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E250CA-2E38-445C-B6B1-D226AA644256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313D9880-DE33-4E6E-9CFA-40E48496106B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="text" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="121">
   <si>
     <t>key</t>
   </si>
@@ -371,6 +371,18 @@
   </si>
   <si>
     <t>Akmenys naudingi statant ar mėtant. Stenkitės neišmesti jų visų, jie yra naudingesni mažiems pastatams.</t>
+  </si>
+  <si>
+    <t>crystal_skill_title</t>
+  </si>
+  <si>
+    <t>crystal_skill_description</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystals are not very stable and are fuel for powerfull ancient weapons. Try to put in on fireplace or jsust to throw it. Lets see what will happened. </t>
   </si>
 </sst>
 </file>
@@ -1234,21 +1246,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="46.140625" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1274,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1276,7 +1288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1312,7 +1324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1323,7 +1335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1345,7 +1357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1356,7 +1368,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1378,7 +1390,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1389,7 +1401,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1400,7 +1412,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -1414,7 +1426,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1425,7 +1437,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -1436,7 +1448,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -1447,7 +1459,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1469,7 +1481,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1480,7 +1492,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1491,7 +1503,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1502,7 +1514,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1513,7 +1525,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1535,7 +1547,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1546,7 +1558,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -1560,7 +1572,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>80</v>
       </c>
@@ -1574,7 +1586,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -1602,73 +1614,101 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="46" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>93</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="47" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>94</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add fire blade skill, polish game
</commit_message>
<xml_diff>
--- a/assets/translation/text.xlsx
+++ b/assets/translation/text.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28814"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\assets\translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313D9880-DE33-4E6E-9CFA-40E48496106B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FF246A5-E64F-468B-983F-45D9D9DCDCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="text" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="187">
   <si>
     <t>key</t>
   </si>
@@ -145,6 +161,18 @@
     <t>Ціна</t>
   </si>
   <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Кількість</t>
+  </si>
+  <si>
+    <t>Kiekis</t>
+  </si>
+  <si>
     <t>skill</t>
   </si>
   <si>
@@ -226,6 +254,15 @@
     <t>Базова ціна</t>
   </si>
   <si>
+    <t>item_type_consumable</t>
+  </si>
+  <si>
+    <t>Consumable</t>
+  </si>
+  <si>
+    <t>item_type_skill</t>
+  </si>
+  <si>
     <t>skill_upgrade</t>
   </si>
   <si>
@@ -253,6 +290,12 @@
     <t>Максимальний рівень</t>
   </si>
   <si>
+    <t>__PLAYER_DAMAGE_SKILLS__</t>
+  </si>
+  <si>
+    <t>spark_skill_t</t>
+  </si>
+  <si>
     <t>Spark</t>
   </si>
   <si>
@@ -262,7 +305,7 @@
     <t>Kibirkštis</t>
   </si>
   <si>
-    <t>spark_skill_description</t>
+    <t>spark_skill_d</t>
   </si>
   <si>
     <t>Spark is esential skill of every wizard. Be like Zeus throw yout sparks on your enemies!</t>
@@ -274,13 +317,97 @@
     <t>Kibirkštis yra pagrindinis kiekvieno mago įgūdis. Būkite kaip Zeusas, meskite kibirkštis į savo priešus!</t>
   </si>
   <si>
-    <t>aim_skill_description</t>
-  </si>
-  <si>
-    <t>spark_skill_title</t>
-  </si>
-  <si>
-    <t>aim_skill_title</t>
+    <t>snowball_skill_t</t>
+  </si>
+  <si>
+    <t>Snowball</t>
+  </si>
+  <si>
+    <t>Сніжок</t>
+  </si>
+  <si>
+    <t>snowball_skill_d</t>
+  </si>
+  <si>
+    <t>Snowball is not a joke, it's powerfull weapon if you know how to use it. It does damage in area and can slow down your enemies. Ymir is helping you to slow down your enemies.</t>
+  </si>
+  <si>
+    <t>fireball_skill_t</t>
+  </si>
+  <si>
+    <t>Fireball</t>
+  </si>
+  <si>
+    <t>fireball_skill_d</t>
+  </si>
+  <si>
+    <t>Fireball. What you expect - it's does damge in area and takes enemies in fire. Agni is proud of you!</t>
+  </si>
+  <si>
+    <t>acid_meteor_skill_t</t>
+  </si>
+  <si>
+    <t>Toxic meteor</t>
+  </si>
+  <si>
+    <t>acid_meteor_skill_d</t>
+  </si>
+  <si>
+    <t>Toxic meteor is  one of the rare meteors which wasn't touch the Earth surface.Powerfull weapon,  after it will contact surface - it's unstably will emit acid gas which damage your enemies.</t>
+  </si>
+  <si>
+    <t>stone_skill_t</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Камінчик</t>
+  </si>
+  <si>
+    <t>Akmenis</t>
+  </si>
+  <si>
+    <t>stone_skill_d</t>
+  </si>
+  <si>
+    <t>Stones are usefull for building or throwing it. Please try not to throw all of them they are more usefull for small buildings.</t>
+  </si>
+  <si>
+    <t>Камінці корисні для будівництва або кидання. Будь ласка, намагайтеся не викидати їх усі, вони більш корисні для невеликих будівель.</t>
+  </si>
+  <si>
+    <t>Akmenys naudingi statant ar mėtant. Stenkitės neišmesti jų visų, jie yra naudingesni mažiems pastatams.</t>
+  </si>
+  <si>
+    <t>crystal_skill_t</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>crystal_skill_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystals are not very stable and are fuel for powerfull ancient weapons. Try to put in on fireplace or just to throw it. Lets see what will happened. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystals are not very stable and are fuel for powerfull ancient weapons. Try to put in on fireplace or jsust to throw it. Lets see what will happened. </t>
+  </si>
+  <si>
+    <t>__PLAYER_DEFFENSIVE_SKILLS__</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>aim_skill_t</t>
   </si>
   <si>
     <t>Zoom in</t>
@@ -289,6 +416,12 @@
     <t>Приближення</t>
   </si>
   <si>
+    <t>Priartinti</t>
+  </si>
+  <si>
+    <t>aim_skill_d</t>
+  </si>
+  <si>
     <t>Allows player to zoom in enemies and other objects. Uses stamina as main resourse. Good to see you enemies from big distances.</t>
   </si>
   <si>
@@ -298,27 +431,108 @@
     <t>Leidžia žaidėjui priartinti priešus ir kitus objektus. Naudoja ištvermę kaip pagrindinį resursą. Smagu matyti jus priešus iš didelių atstumų.</t>
   </si>
   <si>
-    <t>Priartinti</t>
+    <t>dash_skill_t</t>
+  </si>
+  <si>
+    <t>Dash</t>
+  </si>
+  <si>
+    <t>dash_skill_d</t>
+  </si>
+  <si>
+    <t>You can dash through your enemies to avoid damage or move faster. It's a best way to clean up dangeons and stay safe.</t>
+  </si>
+  <si>
+    <t>__PLAYER_CONSUMABLE_BOOST_SKILLS__</t>
+  </si>
+  <si>
+    <t>damage_boost_skill_t</t>
+  </si>
+  <si>
+    <t>Damage boost</t>
+  </si>
+  <si>
+    <t>damage_boost_skill_d</t>
+  </si>
+  <si>
+    <t>This tablet can give you extra power on your skills! But of couse temporary, use it and go find some enemies to test new powers!</t>
+  </si>
+  <si>
+    <t>speed_boost_skill_t</t>
+  </si>
+  <si>
+    <t>Speed up!</t>
+  </si>
+  <si>
+    <t>speed_boost_skill_d</t>
+  </si>
+  <si>
+    <t>Aftrer consumtion this  - you will be unstopable...unstopable faster then before. This item after consumtion gives some extra speed. It impacts a dash and jump as well - more speed, safer you are!</t>
+  </si>
+  <si>
+    <t>heal_skill_t</t>
+  </si>
+  <si>
+    <t>Health recover</t>
+  </si>
+  <si>
+    <t>heal_skill_d</t>
+  </si>
+  <si>
+    <t>Some times we can't avoid much damage, then you can use some extra help from heal tablet. It restores some health points!</t>
+  </si>
+  <si>
+    <t>mana_skill_t</t>
+  </si>
+  <si>
+    <t>Mana recover</t>
+  </si>
+  <si>
+    <t>mana_skill_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take care always about your mana, as it can save your life sometimes. This restores some mana points, so you can have more using it. </t>
+  </si>
+  <si>
+    <t>stamina_skill_t</t>
+  </si>
+  <si>
+    <t>Stamina recover</t>
+  </si>
+  <si>
+    <t>stamina_skill_d</t>
+  </si>
+  <si>
+    <t>Be strong! Sometimes you need to run far or dash more, or use skills which consumes stamina. Consume it to restore some additional amount of stamina.</t>
   </si>
   <si>
     <t>how_to_use_maintainable</t>
   </si>
   <si>
+    <t>Click and hold mouse button when item in hands (LMB for left hand / RMB for right hand).</t>
+  </si>
+  <si>
+    <t>Натисніть і утримуйте кнопку миші, коли предмет у руках (ЛКМ для лівої руки / ПКМ для правої руки).</t>
+  </si>
+  <si>
+    <t>Spustelėkite ir laikykite pelės mygtuką, kai daiktas yra rankose (LMB kairiajai rankai / RMB dešinei rankai).</t>
+  </si>
+  <si>
     <t>how_to_use_click_consumable</t>
   </si>
   <si>
+    <t>Click LMB or RMB to use when item in one of your hands. Item will be consumed after usage!</t>
+  </si>
+  <si>
+    <t>Клацніть ЛКМ або ПКМ, щоб використати предмет у своїх руках. Предмет буде спожито після використання!</t>
+  </si>
+  <si>
+    <t>Spustelėkite LMB arba RMB, kad naudotumėte, kai prekė yra vienoje iš jūsų rankų. Daiktas bus sunaudota po naudojimo!</t>
+  </si>
+  <si>
     <t>how_to_use_click</t>
   </si>
   <si>
-    <t>Click and hold mouse button when item in hands (LMB for left hand / RMB for right hand).</t>
-  </si>
-  <si>
-    <t>Spustelėkite ir laikykite pelės mygtuką, kai daiktas yra rankose (LMB kairiajai rankai / RMB dešinei rankai).</t>
-  </si>
-  <si>
-    <t>Натисніть і утримуйте кнопку миші, коли предмет у руках (ЛКМ для лівої руки / ПКМ для правої руки).</t>
-  </si>
-  <si>
     <t>Click LMB or RMB to use when item in one of your hands.</t>
   </si>
   <si>
@@ -328,68 +542,68 @@
     <t>Spustelėkite LMB arba RMB, kad naudotumėte, kai prekė yra vienoje iš jūsų rankų.</t>
   </si>
   <si>
-    <t>Click LMB or RMB to use when item in one of your hands. Item will be consumed after usage!</t>
-  </si>
-  <si>
-    <t>Клацніть ЛКМ або ПКМ, щоб використати предмет у своїх руках. Предмет буде спожито після використання!</t>
-  </si>
-  <si>
-    <t>Spustelėkite LMB arba RMB, kad naudotumėte, kai prekė yra vienoje iš jūsų rankų. Daiktas bus sunaudota po naudojimo!</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Кількість</t>
-  </si>
-  <si>
-    <t>Kiekis</t>
-  </si>
-  <si>
-    <t>stone_skill_title</t>
-  </si>
-  <si>
-    <t>stone_skill_description</t>
-  </si>
-  <si>
-    <t>Stone</t>
-  </si>
-  <si>
-    <t>Akmenis</t>
-  </si>
-  <si>
-    <t>Камінчик</t>
-  </si>
-  <si>
-    <t>Stones are usefull for building or throwing it. Please try not to throw all of them they are more usefull for small buildings.</t>
-  </si>
-  <si>
-    <t>Камінці корисні для будівництва або кидання. Будь ласка, намагайтеся не викидати їх усі, вони більш корисні для невеликих будівель.</t>
-  </si>
-  <si>
-    <t>Akmenys naudingi statant ar mėtant. Stenkitės neišmesti jų visų, jie yra naudingesni mažiems pastatams.</t>
-  </si>
-  <si>
-    <t>crystal_skill_title</t>
-  </si>
-  <si>
-    <t>crystal_skill_description</t>
-  </si>
-  <si>
-    <t>Crystal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crystals are not very stable and are fuel for powerfull ancient weapons. Try to put in on fireplace or jsust to throw it. Lets see what will happened. </t>
+    <t>__ENUMS___</t>
+  </si>
+  <si>
+    <t>IMMUNE_TO_DAMAGE</t>
+  </si>
+  <si>
+    <t>Damage immunity</t>
+  </si>
+  <si>
+    <t>NO_MANA</t>
+  </si>
+  <si>
+    <t>No enough mana</t>
+  </si>
+  <si>
+    <t>NO_STAMINA</t>
+  </si>
+  <si>
+    <t>No enough stamina</t>
+  </si>
+  <si>
+    <t>LOCK</t>
+  </si>
+  <si>
+    <t>Skill is on lock</t>
+  </si>
+  <si>
+    <t>ON_CD</t>
+  </si>
+  <si>
+    <t>Skill is on cooldown</t>
+  </si>
+  <si>
+    <t>IDLE</t>
+  </si>
+  <si>
+    <t>Skill is iddle</t>
+  </si>
+  <si>
+    <t>FULL_HP</t>
+  </si>
+  <si>
+    <t>Failed cause full health</t>
+  </si>
+  <si>
+    <t>FULL_MANA</t>
+  </si>
+  <si>
+    <t>Failed cause full mana</t>
+  </si>
+  <si>
+    <t>FULL_STAMINA</t>
+  </si>
+  <si>
+    <t>Failed cause full stamina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,6 +737,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -866,9 +1086,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -916,7 +1144,38 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -927,6 +1186,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3BDC87A-5C32-4235-8298-66538B8D2C9E}" name="Table1" displayName="Table1" ref="A87:D89" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A87:D89" xr:uid="{C3BDC87A-5C32-4235-8298-66538B8D2C9E}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{AB3AC377-98B7-4138-ACED-7FB17D359A2A}" name="how_to_use_maintainable"/>
+    <tableColumn id="2" xr3:uid="{041CFDAC-323B-466E-8BC3-FE609ECA6EBD}" name="Click and hold mouse button when item in hands (LMB for left hand / RMB for right hand)." dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0B5FC283-BC32-4B9E-9B83-CD4CC00AA236}" name="Натисніть і утримуйте кнопку миші, коли предмет у руках (ЛКМ для лівої руки / ПКМ для правої руки)." dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{04865A92-F465-4237-BD11-E26AFAC0D825}" name="Spustelėkite ir laikykite pelės mygtuką, kai daiktas yra rankose (LMB kairiajai rankai / RMB dešinei rankai)." dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8EF8E82E-635C-4A09-BE79-77F40AB90C5F}" name="Table2" displayName="Table2" ref="A56:D64" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A56:D64" xr:uid="{8EF8E82E-635C-4A09-BE79-77F40AB90C5F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{21F85E53-C360-4BAF-BAE0-879CD85F559E}" name="__PLAYER_DEFFENSIVE_SKILLS__"/>
+    <tableColumn id="2" xr3:uid="{3E6141C5-C984-4BD8-8699-A412370AF5DA}" name="Column1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{4FC213BA-F1EA-45F8-8DEC-80B4EAA25453}" name="Column2" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{0D43A3D3-B2AB-4EFB-A974-BA6E0026009A}" name="Column3" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1246,21 +1531,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="46.109375" customWidth="1"/>
-    <col min="2" max="2" width="34.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1302,7 +1587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1313,7 +1598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1335,7 +1620,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1346,7 +1631,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1357,7 +1642,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1368,7 +1653,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1379,7 +1664,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1390,7 +1675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1401,7 +1686,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1412,308 +1697,592 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15"/>
+    <row r="28" spans="1:3" ht="15">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15">
+      <c r="A34" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15"/>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="43.15">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="72.75">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15"/>
+    <row r="42" spans="1:4" ht="15">
+      <c r="A42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="43.5">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15"/>
+    <row r="45" spans="1:4" ht="15">
+      <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="72.75">
+      <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="47" spans="1:4" ht="15"/>
+    <row r="48" spans="1:4" ht="15">
+      <c r="A48" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="D48" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="1" t="s">
+    </row>
+    <row r="49" spans="1:4" ht="57.75">
+      <c r="A49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" s="1" t="s">
+    </row>
+    <row r="50" spans="1:4" ht="15"/>
+    <row r="51" spans="1:4" ht="15">
+      <c r="A51" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="C51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="57.75">
+      <c r="A52" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="B52" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15"/>
+    <row r="54" spans="1:4" ht="15"/>
+    <row r="55" spans="1:4" ht="15"/>
+    <row r="56" spans="1:4" ht="15">
+      <c r="A56" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>101</v>
+      <c r="C56" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15"/>
+    <row r="58" spans="1:4" ht="15">
+      <c r="A58" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="57.75">
+      <c r="A59" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15"/>
+    <row r="61" spans="1:4" ht="15">
+      <c r="A61" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="43.5">
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15"/>
+    <row r="64" spans="1:4" ht="15">
+      <c r="A64" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15">
+      <c r="A66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="57.75">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15">
+      <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="72.75">
+      <c r="A70" t="s">
+        <v>142</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15"/>
+    <row r="72" spans="1:2" ht="15">
+      <c r="A72" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="43.5">
+      <c r="A73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15">
+      <c r="A75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="57.75">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15">
+      <c r="A78" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="57.75">
+      <c r="A79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15"/>
+    <row r="84" spans="1:4" ht="15"/>
+    <row r="85" spans="1:4" ht="15"/>
+    <row r="87" spans="1:4" ht="43.5">
+      <c r="A87" t="s">
+        <v>156</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="57.75">
+      <c r="A88" t="s">
+        <v>160</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="43.5">
+      <c r="A89" t="s">
+        <v>164</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15">
+      <c r="A92" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15">
+      <c r="A94" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15">
+      <c r="A95" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15">
+      <c r="A96" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15">
+      <c r="A97" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15">
+      <c r="A98" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15">
+      <c r="A99" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15">
+      <c r="A100" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15">
+      <c r="A101" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15">
+      <c r="A102" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add basic menu, player creation, saving and loading
</commit_message>
<xml_diff>
--- a/assets/translation/text.xlsx
+++ b/assets/translation/text.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28822"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\01_Ivan\01_Godot\tower-dungeon\assets\translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FF246A5-E64F-468B-983F-45D9D9DCDCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E68E65C-ECEC-4281-8E48-4822B126F097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="255">
   <si>
     <t>key</t>
   </si>
@@ -266,19 +266,13 @@
     <t>skill_upgrade</t>
   </si>
   <si>
-    <t>Skill Upgrade</t>
-  </si>
-  <si>
-    <t>Покращення навички</t>
+    <t>Skill upgrade</t>
   </si>
   <si>
     <t>parameter_name</t>
   </si>
   <si>
-    <t>Parameter Name</t>
-  </si>
-  <si>
-    <t>Назва параметру</t>
+    <t>Parameter name</t>
   </si>
   <si>
     <t>max_lvl</t>
@@ -287,7 +281,133 @@
     <t>Max level</t>
   </si>
   <si>
-    <t>Максимальний рівень</t>
+    <t>__MENU_SCREENS__</t>
+  </si>
+  <si>
+    <t>menu_back_btn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back </t>
+  </si>
+  <si>
+    <t>menu_back_to_game_btn</t>
+  </si>
+  <si>
+    <t>Back to game</t>
+  </si>
+  <si>
+    <t>menu_play_btn</t>
+  </si>
+  <si>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>menu_restart_btn</t>
+  </si>
+  <si>
+    <t>Restart</t>
+  </si>
+  <si>
+    <t>menu_properties_btn</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>menu_controls_btn</t>
+  </si>
+  <si>
+    <t>Controls</t>
+  </si>
+  <si>
+    <t>menu_give_up_btn</t>
+  </si>
+  <si>
+    <t>Give up</t>
+  </si>
+  <si>
+    <t>menu_quit_btn</t>
+  </si>
+  <si>
+    <t>Quit game</t>
+  </si>
+  <si>
+    <t>menu_new_game_btn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New </t>
+  </si>
+  <si>
+    <t>menu_continue_game_btn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue </t>
+  </si>
+  <si>
+    <t>easy_difficulty_d</t>
+  </si>
+  <si>
+    <t>The enemies will do less damage to you, also prices will be more easy afordable in shop. Fits for unexperienced players or for those who just want click and have fun (to do just pew-pew with some fireballs)</t>
+  </si>
+  <si>
+    <t>nomal_difficulty_d</t>
+  </si>
+  <si>
+    <t>Classic way to play the game. I tried my best to do balance on this mode, which will allow players  to have fun and in same time not so easy to finish game.</t>
+  </si>
+  <si>
+    <t>hard_difficulty_d</t>
+  </si>
+  <si>
+    <t>More damage taken from enemies, but more drop from them. Fun to try after comliting normal difficulty</t>
+  </si>
+  <si>
+    <t>easy_difficulty_t</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>normal_difficulty_t</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>hard_difficulty_t</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>new_game</t>
+  </si>
+  <si>
+    <t>New Game</t>
+  </si>
+  <si>
+    <t>menu_enter_username_placeholder</t>
+  </si>
+  <si>
+    <t>Please enter your username here</t>
+  </si>
+  <si>
+    <t>select_game_difficulty</t>
+  </si>
+  <si>
+    <t>Please select game difficulty for your character</t>
+  </si>
+  <si>
+    <t>menu_create_new_character_btn</t>
+  </si>
+  <si>
+    <t>Create character</t>
+  </si>
+  <si>
+    <t>continue_game</t>
+  </si>
+  <si>
+    <t>Continue game</t>
   </si>
   <si>
     <t>__PLAYER_DAMAGE_SKILLS__</t>
@@ -344,6 +464,18 @@
     <t>Fireball. What you expect - it's does damge in area and takes enemies in fire. Agni is proud of you!</t>
   </si>
   <si>
+    <t>fire_blade_trap_skill_t</t>
+  </si>
+  <si>
+    <t>Fireblade trap</t>
+  </si>
+  <si>
+    <t>fire_blade_trap_skill_d</t>
+  </si>
+  <si>
+    <t>Fireblade trap - technical and magical in same time. Good to fight against lot of ground enemies. Will turn them at fire. But be carefull and drop it wisely as it could be useless in unexperienced hands.</t>
+  </si>
+  <si>
     <t>acid_meteor_skill_t</t>
   </si>
   <si>
@@ -452,10 +584,22 @@
     <t>Damage boost</t>
   </si>
   <si>
+    <t>Підсилення атаки</t>
+  </si>
+  <si>
+    <t>Žalos padidinimas</t>
+  </si>
+  <si>
     <t>damage_boost_skill_d</t>
   </si>
   <si>
-    <t>This tablet can give you extra power on your skills! But of couse temporary, use it and go find some enemies to test new powers!</t>
+    <t>This tablet can give you extra power on your skills! But of couse temporary, use it and go find some enemies...</t>
+  </si>
+  <si>
+    <t>Ця таблетка тимчасово підсилює твої навички! Використай її та випробуй нову силу на ворогах!</t>
+  </si>
+  <si>
+    <t>Ši tabletė suteikia laikiną galią tavo įgūdžiams! Naudok ją ir išbandyk naujas galias prieš priešus!</t>
   </si>
   <si>
     <t>speed_boost_skill_t</t>
@@ -464,10 +608,22 @@
     <t>Speed up!</t>
   </si>
   <si>
+    <t>Прискорення!</t>
+  </si>
+  <si>
+    <t>Paspartėjimas!</t>
+  </si>
+  <si>
     <t>speed_boost_skill_d</t>
   </si>
   <si>
-    <t>Aftrer consumtion this  - you will be unstopable...unstopable faster then before. This item after consumtion gives some extra speed. It impacts a dash and jump as well - more speed, safer you are!</t>
+    <t>Aftrer consumtion this - you will be unstopable...unstopable faster then before...</t>
+  </si>
+  <si>
+    <t>Після прийому ти станеш невпинним... ще швидшим, ніж раніше. Впливає на ривок і стрибок – більше швидкості, більше безпеки!</t>
+  </si>
+  <si>
+    <t>Po vartojimo būsi nesustabdomas... dar greitesnis nei anksčiau. Tai veikia šuolį ir spurtą – daugiau greičio, daugiau saugumo!</t>
   </si>
   <si>
     <t>heal_skill_t</t>
@@ -476,10 +632,22 @@
     <t>Health recover</t>
   </si>
   <si>
+    <t>Відновлення здоров'я</t>
+  </si>
+  <si>
+    <t>Gyvybės atkūrimas</t>
+  </si>
+  <si>
     <t>heal_skill_d</t>
   </si>
   <si>
-    <t>Some times we can't avoid much damage, then you can use some extra help from heal tablet. It restores some health points!</t>
+    <t>Some times we can't avoid much damage, then you can use some extra help from heal tablet...</t>
+  </si>
+  <si>
+    <t>Іноді уникнути шкоди неможливо, тоді допоможе лікувальна таблетка. Вона відновлює здоров’я!</t>
+  </si>
+  <si>
+    <t>Kartais nepavyksta išvengti žalos – tada padės gydomoji tabletė. Ji atkuria šiek tiek gyvybės taškų!</t>
   </si>
   <si>
     <t>mana_skill_t</t>
@@ -488,10 +656,22 @@
     <t>Mana recover</t>
   </si>
   <si>
+    <t>Відновлення мани</t>
+  </si>
+  <si>
+    <t>Manos atkūrimas</t>
+  </si>
+  <si>
     <t>mana_skill_d</t>
   </si>
   <si>
-    <t xml:space="preserve">Take care always about your mana, as it can save your life sometimes. This restores some mana points, so you can have more using it. </t>
+    <t>Take care always about your mana, as it can save your life sometimes...</t>
+  </si>
+  <si>
+    <t>Завжди слідкуй за маною — вона може врятувати життя. Ця таблетка відновлює ману для використання навичок.</t>
+  </si>
+  <si>
+    <t>Visada rūpinkis mana – ji gali išgelbėti tavo gyvybę. Ši tabletė atkuria šiek tiek manos.</t>
   </si>
   <si>
     <t>stamina_skill_t</t>
@@ -500,10 +680,22 @@
     <t>Stamina recover</t>
   </si>
   <si>
+    <t>Відновлення витривалості</t>
+  </si>
+  <si>
+    <t>Ištvermės atkūrimas</t>
+  </si>
+  <si>
     <t>stamina_skill_d</t>
   </si>
   <si>
-    <t>Be strong! Sometimes you need to run far or dash more, or use skills which consumes stamina. Consume it to restore some additional amount of stamina.</t>
+    <t>Be strong! Sometimes you need to run far or dash more, or use skills which consumes stamina...</t>
+  </si>
+  <si>
+    <t>Будь сильним! Іноді потрібно далеко бігти чи більше використовувати навички, що споживають витривалість. Ця таблетка відновлює її.</t>
+  </si>
+  <si>
+    <t>Būk stiprus! Kartais reikia daugiau bėgti, šuoliuoti ar naudoti įgūdžius, kurie naudoja ištvermę. Ši tabletė ją atkuria.</t>
   </si>
   <si>
     <t>how_to_use_maintainable</t>
@@ -597,6 +789,18 @@
   </si>
   <si>
     <t>Failed cause full stamina</t>
+  </si>
+  <si>
+    <t>error_username_exists</t>
+  </si>
+  <si>
+    <t>Sorry such username already exists, please try another</t>
+  </si>
+  <si>
+    <t>error_username_not_emtpy</t>
+  </si>
+  <si>
+    <t>Oh...sorry but you can't have no name here, you are not like Arya Stark at 6 season.</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1290,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1097,6 +1301,10 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1189,8 +1397,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3BDC87A-5C32-4235-8298-66538B8D2C9E}" name="Table1" displayName="Table1" ref="A87:D89" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A87:D89" xr:uid="{C3BDC87A-5C32-4235-8298-66538B8D2C9E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3BDC87A-5C32-4235-8298-66538B8D2C9E}" name="Table1" displayName="Table1" ref="A126:D128" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A126:D128" xr:uid="{C3BDC87A-5C32-4235-8298-66538B8D2C9E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AB3AC377-98B7-4138-ACED-7FB17D359A2A}" name="how_to_use_maintainable"/>
     <tableColumn id="2" xr3:uid="{041CFDAC-323B-466E-8BC3-FE609ECA6EBD}" name="Click and hold mouse button when item in hands (LMB for left hand / RMB for right hand)." dataDxfId="7"/>
@@ -1202,8 +1410,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8EF8E82E-635C-4A09-BE79-77F40AB90C5F}" name="Table2" displayName="Table2" ref="A56:D64" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A56:D64" xr:uid="{8EF8E82E-635C-4A09-BE79-77F40AB90C5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8EF8E82E-635C-4A09-BE79-77F40AB90C5F}" name="Table2" displayName="Table2" ref="A95:D103" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A95:D103" xr:uid="{8EF8E82E-635C-4A09-BE79-77F40AB90C5F}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{21F85E53-C360-4BAF-BAE0-879CD85F559E}" name="__PLAYER_DEFFENSIVE_SKILLS__"/>
     <tableColumn id="2" xr3:uid="{3E6141C5-C984-4BD8-8699-A412370AF5DA}" name="Column1" dataDxfId="2"/>
@@ -1531,13 +1744,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="46.140625" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
@@ -1546,16 +1759,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1810,102 +2023,109 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15"/>
-    <row r="28" spans="1:3" ht="15">
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="1" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="B33" s="7" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="15">
-      <c r="A34" s="2" t="s">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15"/>
-    <row r="36" spans="1:4">
+      <c r="B34" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="43.15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="1" t="s">
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="15">
+      <c r="B38" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="72.75">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -1913,8 +2133,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15"/>
-    <row r="42" spans="1:4" ht="15">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -1922,7 +2141,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="43.5">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -1930,8 +2149,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15"/>
-    <row r="45" spans="1:4" ht="15">
+    <row r="45" spans="1:3" ht="72.75">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -1939,7 +2157,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="72.75">
+    <row r="46" spans="1:3" ht="57.75">
       <c r="A46" t="s">
         <v>104</v>
       </c>
@@ -1947,334 +2165,570 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15"/>
-    <row r="48" spans="1:4" ht="15">
-      <c r="A48" t="s">
+    <row r="47" spans="1:3" ht="43.5">
+      <c r="A47" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C48" s="1" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="57.75">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
         <v>110</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C49" s="1" t="s">
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>112</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15"/>
-    <row r="51" spans="1:4" ht="15">
-      <c r="A51" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>114</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="57.75">
-      <c r="A52" t="s">
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
         <v>116</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="1" t="s">
+    </row>
+    <row r="55" spans="1:2" ht="29.25">
+      <c r="A55" t="s">
         <v>118</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15"/>
-    <row r="54" spans="1:4" ht="15"/>
-    <row r="55" spans="1:4" ht="15"/>
-    <row r="56" spans="1:4" ht="15">
-      <c r="A56" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="1" t="s">
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
         <v>120</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D56" s="1" t="s">
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="15"/>
-    <row r="58" spans="1:4" ht="15">
-      <c r="A58" t="s">
+      <c r="B59" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="1" t="s">
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="1" t="s">
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
         <v>125</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="57.75">
-      <c r="A59" t="s">
+      <c r="C65" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C59" s="1" t="s">
+    </row>
+    <row r="66" spans="1:4" ht="43.5">
+      <c r="A66" t="s">
         <v>129</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="B66" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="15"/>
-    <row r="61" spans="1:4" ht="15">
-      <c r="A61" t="s">
+      <c r="C66" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="43.5">
-      <c r="A62" t="s">
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
         <v>133</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15"/>
-    <row r="64" spans="1:4" ht="15">
-      <c r="A64" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15">
-      <c r="A66" t="s">
+    <row r="69" spans="1:4" ht="72.75">
+      <c r="A69" t="s">
         <v>136</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="57.75">
-      <c r="A67" t="s">
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
         <v>138</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B71" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15">
-      <c r="A69" t="s">
+    <row r="72" spans="1:4" ht="43.5">
+      <c r="A72" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="72.75">
-      <c r="A70" t="s">
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
         <v>142</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15"/>
-    <row r="72" spans="1:2" ht="15">
-      <c r="A72" t="s">
+    <row r="75" spans="1:4" ht="72.75">
+      <c r="A75" t="s">
         <v>144</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="43.5">
-      <c r="A73" t="s">
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
         <v>146</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B84" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15">
-      <c r="A75" t="s">
+    <row r="85" spans="1:4" ht="72.75">
+      <c r="A85" t="s">
         <v>148</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="57.75">
-      <c r="A76" t="s">
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
         <v>150</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B87" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" ht="15">
-      <c r="A78" t="s">
+      <c r="C87" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="57.75">
-      <c r="A79" t="s">
-        <v>154</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15"/>
-    <row r="84" spans="1:4" ht="15"/>
-    <row r="85" spans="1:4" ht="15"/>
-    <row r="87" spans="1:4" ht="43.5">
-      <c r="A87" t="s">
-        <v>156</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="57.75">
       <c r="A88" t="s">
+        <v>154</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>158</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="57.75">
+      <c r="A91" t="s">
         <v>160</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D91" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="43.5">
-      <c r="A89" t="s">
+      <c r="B95" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C95" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="D95" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D89" s="1" t="s">
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="15">
-      <c r="A92" s="3" t="s">
+      <c r="B97" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="15">
-      <c r="A94" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15">
-      <c r="A95" s="5" t="s">
+    <row r="98" spans="1:4" ht="57.75">
+      <c r="A98" t="s">
         <v>171</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="15">
-      <c r="A96" s="5" t="s">
+      <c r="C98" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="15">
-      <c r="A97" s="5" t="s">
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
         <v>175</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="15">
-      <c r="A98" s="5" t="s">
+    <row r="101" spans="1:4" ht="43.5">
+      <c r="A101" t="s">
         <v>177</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15">
-      <c r="A99" s="4" t="s">
+    <row r="103" spans="1:4">
+      <c r="A103" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B99" s="1" t="s">
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" ht="15">
-      <c r="A100" s="4" t="s">
+      <c r="B105" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="C105" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" ht="15">
-      <c r="A101" s="4" t="s">
+      <c r="D105" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B101" s="1" t="s">
+    </row>
+    <row r="106" spans="1:4" ht="43.5">
+      <c r="A106" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" ht="15">
-      <c r="A102" s="4" t="s">
+      <c r="B106" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="C106" s="1" t="s">
         <v>186</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>188</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="57.75">
+      <c r="A109" t="s">
+        <v>192</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>196</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="43.5">
+      <c r="A112" t="s">
+        <v>200</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>204</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="43.5">
+      <c r="A115" t="s">
+        <v>208</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>212</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="57.75">
+      <c r="A118" t="s">
+        <v>216</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="43.5">
+      <c r="A126" t="s">
+        <v>220</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="57.75">
+      <c r="A127" t="s">
+        <v>224</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="43.5">
+      <c r="A128" t="s">
+        <v>228</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="29.25">
+      <c r="A143" t="s">
+        <v>251</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="43.5">
+      <c r="A144" t="s">
+        <v>253</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>